<commit_message>
Refactor app.py for improved data handling and validation
- Removed unused imports and added type annotations for better clarity.
- Introduced RLock for thread-safe access to user data store.
- Enhanced user data retrieval and storage functions with locking mechanisms.
- Improved error handling and validation in file parsing and data import processes.
- Refactored inventory item creation and related calculations for better readability and maintainability.
- Added canonical column definitions and header aliases for consistent data processing.
- Updated simulation functions to ensure proper type handling and safety checks.
- Improved graph update logic to handle empty item lists gracefully.
- Enhanced user feedback messages for better clarity during data import and processing.
- Clarified Example.xlsx column names.
</commit_message>
<xml_diff>
--- a/Example.xlsx
+++ b/Example.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\IMSim\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C92C5B2-F267-4F5F-B1BD-3545519D8BFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A810CCE6-DBDB-4B90-8BB2-B578854BD1D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40470" yWindow="1935" windowWidth="23010" windowHeight="13650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="26010" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,12 +27,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
-    <t>Usage Rate</t>
-  </si>
-  <si>
-    <t>Lead Time</t>
-  </si>
-  <si>
     <t>Item Cost</t>
   </si>
   <si>
@@ -46,6 +40,12 @@
   </si>
   <si>
     <t>Hits Per Month</t>
+  </si>
+  <si>
+    <t>Usage Rate (Per Month)</t>
+  </si>
+  <si>
+    <t>Lead Time (Days)</t>
   </si>
 </sst>
 </file>
@@ -104,8 +104,8 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FD565C9C-0FC4-4B36-812E-1A92D0D07C6B}" name="Table1" displayName="Table1" ref="A1:G4" totalsRowShown="0">
   <autoFilter ref="A1:G4" xr:uid="{FD565C9C-0FC4-4B36-812E-1A92D0D07C6B}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{C207A29A-1002-4B6C-ACD4-FCE9735B66D2}" name="Usage Rate"/>
-    <tableColumn id="2" xr3:uid="{006A1EA4-77C8-4A0B-BB9D-8114182AD93A}" name="Lead Time"/>
+    <tableColumn id="1" xr3:uid="{C207A29A-1002-4B6C-ACD4-FCE9735B66D2}" name="Usage Rate (Per Month)"/>
+    <tableColumn id="2" xr3:uid="{006A1EA4-77C8-4A0B-BB9D-8114182AD93A}" name="Lead Time (Days)"/>
     <tableColumn id="3" xr3:uid="{7E3EC65E-7D27-496D-9E1C-020770B59FE9}" name="Item Cost"/>
     <tableColumn id="4" xr3:uid="{E80F8765-8563-4687-8EB9-00C39009DD8F}" name="Initial PNA"/>
     <tableColumn id="5" xr3:uid="{4235FC8D-066D-414F-9134-FB33A89DE586}" name="Safety Allowance (%)"/>
@@ -381,14 +381,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22.28515625" bestFit="1" customWidth="1"/>
@@ -398,25 +396,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>